<commit_message>
Modified the FY13 milestones sheet
Signed-off-by: Zeid Kootbally <zeid.kootbally@nist.gov>

Former-commit-id: 3dba8c3191e4c250c7fb22be9439abfca856c06b
</commit_message>
<xml_diff>
--- a/Management/FY2013/Task-Tracking.xlsx
+++ b/Management/FY2013/Task-Tracking.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17980" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19320" windowHeight="15480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="1" r:id="rId1"/>
@@ -938,30 +938,6 @@
     <xf numFmtId="2" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1020,6 +996,30 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="23">
@@ -1049,6 +1049,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1377,56 +1382,56 @@
   <dimension ref="A1:AF47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30" customWidth="1"/>
-    <col min="2" max="2" width="7.1640625" style="28" customWidth="1"/>
+    <col min="2" max="2" width="7.125" style="20" customWidth="1"/>
     <col min="3" max="3" width="11.5" customWidth="1"/>
     <col min="4" max="4" width="10" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" style="35" customWidth="1"/>
-    <col min="6" max="6" width="25.6640625" customWidth="1"/>
-    <col min="7" max="7" width="7.5" style="28" customWidth="1"/>
-    <col min="8" max="8" width="6.1640625" customWidth="1"/>
-    <col min="9" max="9" width="10.1640625" customWidth="1"/>
-    <col min="10" max="10" width="10.83203125" style="35"/>
-    <col min="11" max="11" width="27.1640625" customWidth="1"/>
-    <col min="12" max="12" width="7.83203125" style="28" customWidth="1"/>
-    <col min="13" max="13" width="6.83203125" customWidth="1"/>
-    <col min="14" max="14" width="10.1640625" customWidth="1"/>
-    <col min="15" max="15" width="11" style="35" customWidth="1"/>
+    <col min="5" max="5" width="11.375" style="27" customWidth="1"/>
+    <col min="6" max="6" width="25.625" customWidth="1"/>
+    <col min="7" max="7" width="7.5" style="20" customWidth="1"/>
+    <col min="8" max="8" width="6.125" customWidth="1"/>
+    <col min="9" max="9" width="10.125" customWidth="1"/>
+    <col min="10" max="10" width="10.875" style="27"/>
+    <col min="11" max="11" width="27.125" customWidth="1"/>
+    <col min="12" max="12" width="7.875" style="20" customWidth="1"/>
+    <col min="13" max="13" width="6.875" customWidth="1"/>
+    <col min="14" max="14" width="10.125" customWidth="1"/>
+    <col min="15" max="15" width="11" style="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="14" t="s">
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="16" t="s">
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
-      <c r="O1" s="18"/>
-    </row>
-    <row r="2" spans="1:32" ht="45">
+      <c r="L1" s="38"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="38"/>
+      <c r="O1" s="39"/>
+    </row>
+    <row r="2" spans="1:32" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="21" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -1435,13 +1440,13 @@
       <c r="D2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="32" t="s">
+      <c r="E2" s="24" t="s">
         <v>4</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="25" t="s">
+      <c r="G2" s="17" t="s">
         <v>2</v>
       </c>
       <c r="H2" s="6" t="s">
@@ -1450,13 +1455,13 @@
       <c r="I2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="36" t="s">
+      <c r="J2" s="28" t="s">
         <v>4</v>
       </c>
       <c r="K2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="L2" s="30" t="s">
+      <c r="L2" s="22" t="s">
         <v>2</v>
       </c>
       <c r="M2" s="9" t="s">
@@ -1465,7 +1470,7 @@
       <c r="N2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="O2" s="38" t="s">
+      <c r="O2" s="30" t="s">
         <v>4</v>
       </c>
       <c r="P2" s="1"/>
@@ -1486,40 +1491,40 @@
       <c r="AE2" s="1"/>
       <c r="AF2" s="1"/>
     </row>
-    <row r="3" spans="1:32" ht="45">
+    <row r="3" spans="1:32" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="24">
+      <c r="B3" s="16">
         <v>1</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="E3" s="33"/>
+      <c r="E3" s="25"/>
       <c r="F3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="26">
+      <c r="G3" s="18">
         <v>2</v>
       </c>
       <c r="H3" s="7"/>
       <c r="I3" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="J3" s="37"/>
+      <c r="J3" s="29"/>
       <c r="K3" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="L3" s="31">
+      <c r="L3" s="23">
         <v>3</v>
       </c>
       <c r="M3" s="10"/>
       <c r="N3" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="O3" s="39"/>
+      <c r="O3" s="31"/>
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
@@ -1538,11 +1543,11 @@
       <c r="AE3" s="1"/>
       <c r="AF3" s="1"/>
     </row>
-    <row r="4" spans="1:32" ht="45">
+    <row r="4" spans="1:32" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="16" t="s">
         <v>22</v>
       </c>
       <c r="C4" s="4" t="s">
@@ -1551,29 +1556,29 @@
       <c r="D4" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="E4" s="33"/>
+      <c r="E4" s="25"/>
       <c r="F4" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="26" t="s">
+      <c r="G4" s="18" t="s">
         <v>22</v>
       </c>
       <c r="H4" s="7"/>
       <c r="I4" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="J4" s="37"/>
+      <c r="J4" s="29"/>
       <c r="K4" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="L4" s="31">
+      <c r="L4" s="23">
         <v>4</v>
       </c>
       <c r="M4" s="10"/>
       <c r="N4" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="O4" s="39"/>
+      <c r="O4" s="31"/>
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
@@ -1592,11 +1597,11 @@
       <c r="AE4" s="1"/>
       <c r="AF4" s="1"/>
     </row>
-    <row r="5" spans="1:32" ht="60">
+    <row r="5" spans="1:32" ht="63" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="16" t="s">
         <v>22</v>
       </c>
       <c r="C5" s="4" t="s">
@@ -1605,29 +1610,31 @@
       <c r="D5" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="E5" s="33"/>
+      <c r="E5" s="25"/>
       <c r="F5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="26">
+      <c r="G5" s="18">
         <v>3</v>
       </c>
       <c r="H5" s="7"/>
       <c r="I5" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="J5" s="37"/>
+      <c r="J5" s="29">
+        <v>41364</v>
+      </c>
       <c r="K5" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="L5" s="31">
+      <c r="L5" s="23">
         <v>2</v>
       </c>
       <c r="M5" s="10"/>
       <c r="N5" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="O5" s="39"/>
+      <c r="O5" s="31"/>
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
@@ -1646,11 +1653,11 @@
       <c r="AE5" s="1"/>
       <c r="AF5" s="1"/>
     </row>
-    <row r="6" spans="1:32" ht="45">
+    <row r="6" spans="1:32" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="24" t="s">
+      <c r="B6" s="16" t="s">
         <v>22</v>
       </c>
       <c r="C6" s="4" t="s">
@@ -1659,29 +1666,31 @@
       <c r="D6" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="E6" s="33"/>
+      <c r="E6" s="25"/>
       <c r="F6" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="26">
+      <c r="G6" s="18">
         <v>1</v>
       </c>
       <c r="H6" s="7"/>
       <c r="I6" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="J6" s="37"/>
+      <c r="J6" s="29">
+        <v>41364</v>
+      </c>
       <c r="K6" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="L6" s="31">
+      <c r="L6" s="23">
         <v>1</v>
       </c>
       <c r="M6" s="10"/>
       <c r="N6" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="O6" s="39"/>
+      <c r="O6" s="31"/>
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
@@ -1700,11 +1709,11 @@
       <c r="AE6" s="1"/>
       <c r="AF6" s="1"/>
     </row>
-    <row r="7" spans="1:32" ht="60">
+    <row r="7" spans="1:32" ht="63" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B7" s="24" t="s">
+      <c r="B7" s="16" t="s">
         <v>22</v>
       </c>
       <c r="C7" s="4" t="s">
@@ -1713,29 +1722,31 @@
       <c r="D7" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="E7" s="33"/>
+      <c r="E7" s="25"/>
       <c r="F7" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="G7" s="26">
-        <v>4</v>
+      <c r="G7" s="18">
+        <v>1</v>
       </c>
       <c r="H7" s="7"/>
       <c r="I7" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="J7" s="37"/>
+      <c r="J7" s="29">
+        <v>41338</v>
+      </c>
       <c r="K7" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="L7" s="31">
+      <c r="L7" s="23">
         <v>5</v>
       </c>
       <c r="M7" s="10"/>
       <c r="N7" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="O7" s="39"/>
+      <c r="O7" s="31"/>
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
@@ -1754,11 +1765,11 @@
       <c r="AE7" s="1"/>
       <c r="AF7" s="1"/>
     </row>
-    <row r="8" spans="1:32" ht="45">
+    <row r="8" spans="1:32" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="16" t="s">
         <v>22</v>
       </c>
       <c r="C8" s="4" t="s">
@@ -1767,17 +1778,17 @@
       <c r="D8" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="E8" s="33"/>
+      <c r="E8" s="25"/>
       <c r="F8" s="7"/>
-      <c r="G8" s="26"/>
+      <c r="G8" s="18"/>
       <c r="H8" s="7"/>
       <c r="I8" s="7"/>
-      <c r="J8" s="37"/>
+      <c r="J8" s="29"/>
       <c r="K8" s="10"/>
-      <c r="L8" s="31"/>
+      <c r="L8" s="23"/>
       <c r="M8" s="10"/>
       <c r="N8" s="10"/>
-      <c r="O8" s="39"/>
+      <c r="O8" s="31"/>
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
@@ -1796,28 +1807,28 @@
       <c r="AE8" s="1"/>
       <c r="AF8" s="1"/>
     </row>
-    <row r="9" spans="1:32" ht="75">
+    <row r="9" spans="1:32" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B9" s="24">
+      <c r="B9" s="16">
         <v>5</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="E9" s="33"/>
+      <c r="E9" s="25"/>
       <c r="F9" s="7"/>
-      <c r="G9" s="26"/>
+      <c r="G9" s="18"/>
       <c r="H9" s="7"/>
       <c r="I9" s="7"/>
-      <c r="J9" s="37"/>
+      <c r="J9" s="29"/>
       <c r="K9" s="10"/>
-      <c r="L9" s="31"/>
+      <c r="L9" s="23"/>
       <c r="M9" s="10"/>
       <c r="N9" s="10"/>
-      <c r="O9" s="39"/>
+      <c r="O9" s="31"/>
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
@@ -1836,11 +1847,11 @@
       <c r="AE9" s="1"/>
       <c r="AF9" s="1"/>
     </row>
-    <row r="10" spans="1:32" ht="75">
+    <row r="10" spans="1:32" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="24">
+      <c r="B10" s="16">
         <v>2</v>
       </c>
       <c r="C10" s="4" t="s">
@@ -1849,17 +1860,17 @@
       <c r="D10" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="E10" s="33"/>
+      <c r="E10" s="25"/>
       <c r="F10" s="7"/>
-      <c r="G10" s="26"/>
+      <c r="G10" s="18"/>
       <c r="H10" s="7"/>
       <c r="I10" s="7"/>
-      <c r="J10" s="37"/>
+      <c r="J10" s="29"/>
       <c r="K10" s="10"/>
-      <c r="L10" s="31"/>
+      <c r="L10" s="23"/>
       <c r="M10" s="10"/>
       <c r="N10" s="10"/>
-      <c r="O10" s="39"/>
+      <c r="O10" s="31"/>
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
@@ -1878,28 +1889,28 @@
       <c r="AE10" s="1"/>
       <c r="AF10" s="1"/>
     </row>
-    <row r="11" spans="1:32" ht="30">
+    <row r="11" spans="1:32" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="24">
+      <c r="B11" s="16">
         <v>3</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="E11" s="33"/>
+      <c r="E11" s="25"/>
       <c r="F11" s="7"/>
-      <c r="G11" s="26"/>
+      <c r="G11" s="18"/>
       <c r="H11" s="7"/>
       <c r="I11" s="7"/>
-      <c r="J11" s="37"/>
+      <c r="J11" s="29"/>
       <c r="K11" s="10"/>
-      <c r="L11" s="31"/>
+      <c r="L11" s="23"/>
       <c r="M11" s="10"/>
       <c r="N11" s="10"/>
-      <c r="O11" s="39"/>
+      <c r="O11" s="31"/>
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
@@ -1918,30 +1929,30 @@
       <c r="AE11" s="1"/>
       <c r="AF11" s="1"/>
     </row>
-    <row r="12" spans="1:32">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="24">
+      <c r="B12" s="16">
         <v>4</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="E12" s="33">
+      <c r="E12" s="25">
         <v>41340</v>
       </c>
       <c r="F12" s="7"/>
-      <c r="G12" s="26"/>
+      <c r="G12" s="18"/>
       <c r="H12" s="7"/>
       <c r="I12" s="7"/>
-      <c r="J12" s="37"/>
+      <c r="J12" s="29"/>
       <c r="K12" s="10"/>
-      <c r="L12" s="31"/>
+      <c r="L12" s="23"/>
       <c r="M12" s="10"/>
       <c r="N12" s="10"/>
-      <c r="O12" s="39"/>
+      <c r="O12" s="31"/>
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
       <c r="R12" s="1"/>
@@ -1960,22 +1971,22 @@
       <c r="AE12" s="1"/>
       <c r="AF12" s="1"/>
     </row>
-    <row r="13" spans="1:32">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
-      <c r="B13" s="24"/>
+      <c r="B13" s="16"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
-      <c r="E13" s="33"/>
+      <c r="E13" s="25"/>
       <c r="F13" s="7"/>
-      <c r="G13" s="26"/>
+      <c r="G13" s="18"/>
       <c r="H13" s="7"/>
       <c r="I13" s="7"/>
-      <c r="J13" s="37"/>
+      <c r="J13" s="29"/>
       <c r="K13" s="10"/>
-      <c r="L13" s="31"/>
+      <c r="L13" s="23"/>
       <c r="M13" s="10"/>
       <c r="N13" s="10"/>
-      <c r="O13" s="39"/>
+      <c r="O13" s="31"/>
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
       <c r="R13" s="1"/>
@@ -1994,22 +2005,22 @@
       <c r="AE13" s="1"/>
       <c r="AF13" s="1"/>
     </row>
-    <row r="14" spans="1:32">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
-      <c r="B14" s="24"/>
+      <c r="B14" s="16"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
-      <c r="E14" s="33"/>
+      <c r="E14" s="25"/>
       <c r="F14" s="7"/>
-      <c r="G14" s="26"/>
+      <c r="G14" s="18"/>
       <c r="H14" s="7"/>
       <c r="I14" s="7"/>
-      <c r="J14" s="37"/>
+      <c r="J14" s="29"/>
       <c r="K14" s="10"/>
-      <c r="L14" s="31"/>
+      <c r="L14" s="23"/>
       <c r="M14" s="10"/>
       <c r="N14" s="10"/>
-      <c r="O14" s="39"/>
+      <c r="O14" s="31"/>
       <c r="P14" s="1"/>
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
@@ -2028,22 +2039,22 @@
       <c r="AE14" s="1"/>
       <c r="AF14" s="1"/>
     </row>
-    <row r="15" spans="1:32">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
-      <c r="B15" s="24"/>
+      <c r="B15" s="16"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
-      <c r="E15" s="33"/>
+      <c r="E15" s="25"/>
       <c r="F15" s="7"/>
-      <c r="G15" s="26"/>
+      <c r="G15" s="18"/>
       <c r="H15" s="7"/>
       <c r="I15" s="7"/>
-      <c r="J15" s="37"/>
+      <c r="J15" s="29"/>
       <c r="K15" s="10"/>
-      <c r="L15" s="31"/>
+      <c r="L15" s="23"/>
       <c r="M15" s="10"/>
       <c r="N15" s="10"/>
-      <c r="O15" s="39"/>
+      <c r="O15" s="31"/>
       <c r="P15" s="1"/>
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
@@ -2062,22 +2073,22 @@
       <c r="AE15" s="1"/>
       <c r="AF15" s="1"/>
     </row>
-    <row r="16" spans="1:32">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
-      <c r="B16" s="24"/>
+      <c r="B16" s="16"/>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
-      <c r="E16" s="33"/>
+      <c r="E16" s="25"/>
       <c r="F16" s="7"/>
-      <c r="G16" s="26"/>
+      <c r="G16" s="18"/>
       <c r="H16" s="7"/>
       <c r="I16" s="7"/>
-      <c r="J16" s="37"/>
+      <c r="J16" s="29"/>
       <c r="K16" s="10"/>
-      <c r="L16" s="31"/>
+      <c r="L16" s="23"/>
       <c r="M16" s="10"/>
       <c r="N16" s="10"/>
-      <c r="O16" s="39"/>
+      <c r="O16" s="31"/>
       <c r="P16" s="1"/>
       <c r="Q16" s="1"/>
       <c r="R16" s="1"/>
@@ -2096,22 +2107,22 @@
       <c r="AE16" s="1"/>
       <c r="AF16" s="1"/>
     </row>
-    <row r="17" spans="1:32">
+    <row r="17" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
-      <c r="B17" s="24"/>
+      <c r="B17" s="16"/>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
-      <c r="E17" s="33"/>
+      <c r="E17" s="25"/>
       <c r="F17" s="7"/>
-      <c r="G17" s="26"/>
+      <c r="G17" s="18"/>
       <c r="H17" s="7"/>
       <c r="I17" s="7"/>
-      <c r="J17" s="37"/>
+      <c r="J17" s="29"/>
       <c r="K17" s="10"/>
-      <c r="L17" s="31"/>
+      <c r="L17" s="23"/>
       <c r="M17" s="10"/>
       <c r="N17" s="10"/>
-      <c r="O17" s="39"/>
+      <c r="O17" s="31"/>
       <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
       <c r="R17" s="1"/>
@@ -2130,22 +2141,22 @@
       <c r="AE17" s="1"/>
       <c r="AF17" s="1"/>
     </row>
-    <row r="18" spans="1:32">
+    <row r="18" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
-      <c r="B18" s="24"/>
+      <c r="B18" s="16"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
-      <c r="E18" s="33"/>
+      <c r="E18" s="25"/>
       <c r="F18" s="7"/>
-      <c r="G18" s="26"/>
+      <c r="G18" s="18"/>
       <c r="H18" s="7"/>
       <c r="I18" s="7"/>
-      <c r="J18" s="37"/>
+      <c r="J18" s="29"/>
       <c r="K18" s="10"/>
-      <c r="L18" s="31"/>
+      <c r="L18" s="23"/>
       <c r="M18" s="10"/>
       <c r="N18" s="10"/>
-      <c r="O18" s="39"/>
+      <c r="O18" s="31"/>
       <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
       <c r="R18" s="1"/>
@@ -2164,22 +2175,22 @@
       <c r="AE18" s="1"/>
       <c r="AF18" s="1"/>
     </row>
-    <row r="19" spans="1:32">
+    <row r="19" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
-      <c r="B19" s="24"/>
+      <c r="B19" s="16"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
-      <c r="E19" s="33"/>
+      <c r="E19" s="25"/>
       <c r="F19" s="7"/>
-      <c r="G19" s="26"/>
+      <c r="G19" s="18"/>
       <c r="H19" s="7"/>
       <c r="I19" s="7"/>
-      <c r="J19" s="37"/>
+      <c r="J19" s="29"/>
       <c r="K19" s="10"/>
-      <c r="L19" s="31"/>
+      <c r="L19" s="23"/>
       <c r="M19" s="10"/>
       <c r="N19" s="10"/>
-      <c r="O19" s="39"/>
+      <c r="O19" s="31"/>
       <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
@@ -2198,22 +2209,22 @@
       <c r="AE19" s="1"/>
       <c r="AF19" s="1"/>
     </row>
-    <row r="20" spans="1:32">
+    <row r="20" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
-      <c r="B20" s="24"/>
+      <c r="B20" s="16"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
-      <c r="E20" s="33"/>
+      <c r="E20" s="25"/>
       <c r="F20" s="7"/>
-      <c r="G20" s="26"/>
+      <c r="G20" s="18"/>
       <c r="H20" s="7"/>
       <c r="I20" s="7"/>
-      <c r="J20" s="37"/>
+      <c r="J20" s="29"/>
       <c r="K20" s="10"/>
-      <c r="L20" s="31"/>
+      <c r="L20" s="23"/>
       <c r="M20" s="10"/>
       <c r="N20" s="10"/>
-      <c r="O20" s="39"/>
+      <c r="O20" s="31"/>
       <c r="P20" s="1"/>
       <c r="Q20" s="1"/>
       <c r="R20" s="1"/>
@@ -2232,22 +2243,22 @@
       <c r="AE20" s="1"/>
       <c r="AF20" s="1"/>
     </row>
-    <row r="21" spans="1:32">
+    <row r="21" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
-      <c r="B21" s="24"/>
+      <c r="B21" s="16"/>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
-      <c r="E21" s="33"/>
+      <c r="E21" s="25"/>
       <c r="F21" s="7"/>
-      <c r="G21" s="26"/>
+      <c r="G21" s="18"/>
       <c r="H21" s="7"/>
       <c r="I21" s="7"/>
-      <c r="J21" s="37"/>
+      <c r="J21" s="29"/>
       <c r="K21" s="10"/>
-      <c r="L21" s="31"/>
+      <c r="L21" s="23"/>
       <c r="M21" s="10"/>
       <c r="N21" s="10"/>
-      <c r="O21" s="39"/>
+      <c r="O21" s="31"/>
       <c r="P21" s="1"/>
       <c r="Q21" s="1"/>
       <c r="R21" s="1"/>
@@ -2266,22 +2277,22 @@
       <c r="AE21" s="1"/>
       <c r="AF21" s="1"/>
     </row>
-    <row r="22" spans="1:32">
+    <row r="22" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
-      <c r="B22" s="24"/>
+      <c r="B22" s="16"/>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
-      <c r="E22" s="33"/>
+      <c r="E22" s="25"/>
       <c r="F22" s="7"/>
-      <c r="G22" s="26"/>
+      <c r="G22" s="18"/>
       <c r="H22" s="7"/>
       <c r="I22" s="7"/>
-      <c r="J22" s="37"/>
+      <c r="J22" s="29"/>
       <c r="K22" s="10"/>
-      <c r="L22" s="31"/>
+      <c r="L22" s="23"/>
       <c r="M22" s="10"/>
       <c r="N22" s="10"/>
-      <c r="O22" s="39"/>
+      <c r="O22" s="31"/>
       <c r="P22" s="1"/>
       <c r="Q22" s="1"/>
       <c r="R22" s="1"/>
@@ -2300,22 +2311,22 @@
       <c r="AE22" s="1"/>
       <c r="AF22" s="1"/>
     </row>
-    <row r="23" spans="1:32">
+    <row r="23" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
-      <c r="B23" s="24"/>
+      <c r="B23" s="16"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
-      <c r="E23" s="33"/>
+      <c r="E23" s="25"/>
       <c r="F23" s="7"/>
-      <c r="G23" s="26"/>
+      <c r="G23" s="18"/>
       <c r="H23" s="7"/>
       <c r="I23" s="7"/>
-      <c r="J23" s="37"/>
+      <c r="J23" s="29"/>
       <c r="K23" s="10"/>
-      <c r="L23" s="31"/>
+      <c r="L23" s="23"/>
       <c r="M23" s="10"/>
       <c r="N23" s="10"/>
-      <c r="O23" s="39"/>
+      <c r="O23" s="31"/>
       <c r="P23" s="1"/>
       <c r="Q23" s="1"/>
       <c r="R23" s="1"/>
@@ -2334,22 +2345,22 @@
       <c r="AE23" s="1"/>
       <c r="AF23" s="1"/>
     </row>
-    <row r="24" spans="1:32">
+    <row r="24" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
-      <c r="B24" s="24"/>
+      <c r="B24" s="16"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
-      <c r="E24" s="33"/>
+      <c r="E24" s="25"/>
       <c r="F24" s="7"/>
-      <c r="G24" s="26"/>
+      <c r="G24" s="18"/>
       <c r="H24" s="7"/>
       <c r="I24" s="7"/>
-      <c r="J24" s="37"/>
+      <c r="J24" s="29"/>
       <c r="K24" s="10"/>
-      <c r="L24" s="31"/>
+      <c r="L24" s="23"/>
       <c r="M24" s="10"/>
       <c r="N24" s="10"/>
-      <c r="O24" s="39"/>
+      <c r="O24" s="31"/>
       <c r="P24" s="1"/>
       <c r="Q24" s="1"/>
       <c r="R24" s="1"/>
@@ -2368,22 +2379,22 @@
       <c r="AE24" s="1"/>
       <c r="AF24" s="1"/>
     </row>
-    <row r="25" spans="1:32">
+    <row r="25" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
-      <c r="B25" s="24"/>
+      <c r="B25" s="16"/>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
-      <c r="E25" s="33"/>
+      <c r="E25" s="25"/>
       <c r="F25" s="7"/>
-      <c r="G25" s="26"/>
+      <c r="G25" s="18"/>
       <c r="H25" s="7"/>
       <c r="I25" s="7"/>
-      <c r="J25" s="37"/>
+      <c r="J25" s="29"/>
       <c r="K25" s="10"/>
-      <c r="L25" s="31"/>
+      <c r="L25" s="23"/>
       <c r="M25" s="10"/>
       <c r="N25" s="10"/>
-      <c r="O25" s="39"/>
+      <c r="O25" s="31"/>
       <c r="P25" s="1"/>
       <c r="Q25" s="1"/>
       <c r="R25" s="1"/>
@@ -2402,22 +2413,22 @@
       <c r="AE25" s="1"/>
       <c r="AF25" s="1"/>
     </row>
-    <row r="26" spans="1:32">
+    <row r="26" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
-      <c r="B26" s="24"/>
+      <c r="B26" s="16"/>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
-      <c r="E26" s="33"/>
+      <c r="E26" s="25"/>
       <c r="F26" s="7"/>
-      <c r="G26" s="26"/>
+      <c r="G26" s="18"/>
       <c r="H26" s="7"/>
       <c r="I26" s="7"/>
-      <c r="J26" s="37"/>
+      <c r="J26" s="29"/>
       <c r="K26" s="10"/>
-      <c r="L26" s="31"/>
+      <c r="L26" s="23"/>
       <c r="M26" s="10"/>
       <c r="N26" s="10"/>
-      <c r="O26" s="39"/>
+      <c r="O26" s="31"/>
       <c r="P26" s="1"/>
       <c r="Q26" s="1"/>
       <c r="R26" s="1"/>
@@ -2436,22 +2447,22 @@
       <c r="AE26" s="1"/>
       <c r="AF26" s="1"/>
     </row>
-    <row r="27" spans="1:32">
+    <row r="27" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
-      <c r="B27" s="24"/>
+      <c r="B27" s="16"/>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
-      <c r="E27" s="33"/>
+      <c r="E27" s="25"/>
       <c r="F27" s="7"/>
-      <c r="G27" s="26"/>
+      <c r="G27" s="18"/>
       <c r="H27" s="7"/>
       <c r="I27" s="7"/>
-      <c r="J27" s="37"/>
+      <c r="J27" s="29"/>
       <c r="K27" s="10"/>
-      <c r="L27" s="31"/>
+      <c r="L27" s="23"/>
       <c r="M27" s="10"/>
       <c r="N27" s="10"/>
-      <c r="O27" s="39"/>
+      <c r="O27" s="31"/>
       <c r="P27" s="1"/>
       <c r="Q27" s="1"/>
       <c r="R27" s="1"/>
@@ -2470,22 +2481,22 @@
       <c r="AE27" s="1"/>
       <c r="AF27" s="1"/>
     </row>
-    <row r="28" spans="1:32">
+    <row r="28" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
-      <c r="B28" s="24"/>
+      <c r="B28" s="16"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
-      <c r="E28" s="33"/>
+      <c r="E28" s="25"/>
       <c r="F28" s="7"/>
-      <c r="G28" s="26"/>
+      <c r="G28" s="18"/>
       <c r="H28" s="7"/>
       <c r="I28" s="7"/>
-      <c r="J28" s="37"/>
+      <c r="J28" s="29"/>
       <c r="K28" s="10"/>
-      <c r="L28" s="31"/>
+      <c r="L28" s="23"/>
       <c r="M28" s="10"/>
       <c r="N28" s="10"/>
-      <c r="O28" s="39"/>
+      <c r="O28" s="31"/>
       <c r="P28" s="1"/>
       <c r="Q28" s="1"/>
       <c r="R28" s="1"/>
@@ -2504,22 +2515,22 @@
       <c r="AE28" s="1"/>
       <c r="AF28" s="1"/>
     </row>
-    <row r="29" spans="1:32">
+    <row r="29" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
-      <c r="B29" s="24"/>
+      <c r="B29" s="16"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
-      <c r="E29" s="33"/>
+      <c r="E29" s="25"/>
       <c r="F29" s="7"/>
-      <c r="G29" s="26"/>
+      <c r="G29" s="18"/>
       <c r="H29" s="7"/>
       <c r="I29" s="7"/>
-      <c r="J29" s="37"/>
+      <c r="J29" s="29"/>
       <c r="K29" s="10"/>
-      <c r="L29" s="31"/>
+      <c r="L29" s="23"/>
       <c r="M29" s="10"/>
       <c r="N29" s="10"/>
-      <c r="O29" s="39"/>
+      <c r="O29" s="31"/>
       <c r="P29" s="1"/>
       <c r="Q29" s="1"/>
       <c r="R29" s="1"/>
@@ -2538,22 +2549,22 @@
       <c r="AE29" s="1"/>
       <c r="AF29" s="1"/>
     </row>
-    <row r="30" spans="1:32">
+    <row r="30" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
-      <c r="B30" s="24"/>
+      <c r="B30" s="16"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
-      <c r="E30" s="33"/>
+      <c r="E30" s="25"/>
       <c r="F30" s="7"/>
-      <c r="G30" s="26"/>
+      <c r="G30" s="18"/>
       <c r="H30" s="7"/>
       <c r="I30" s="7"/>
-      <c r="J30" s="37"/>
+      <c r="J30" s="29"/>
       <c r="K30" s="10"/>
-      <c r="L30" s="31"/>
+      <c r="L30" s="23"/>
       <c r="M30" s="10"/>
       <c r="N30" s="10"/>
-      <c r="O30" s="39"/>
+      <c r="O30" s="31"/>
       <c r="P30" s="1"/>
       <c r="Q30" s="1"/>
       <c r="R30" s="1"/>
@@ -2572,22 +2583,22 @@
       <c r="AE30" s="1"/>
       <c r="AF30" s="1"/>
     </row>
-    <row r="31" spans="1:32">
+    <row r="31" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
-      <c r="B31" s="24"/>
+      <c r="B31" s="16"/>
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
-      <c r="E31" s="33"/>
+      <c r="E31" s="25"/>
       <c r="F31" s="7"/>
-      <c r="G31" s="26"/>
+      <c r="G31" s="18"/>
       <c r="H31" s="7"/>
       <c r="I31" s="7"/>
-      <c r="J31" s="37"/>
+      <c r="J31" s="29"/>
       <c r="K31" s="10"/>
-      <c r="L31" s="31"/>
+      <c r="L31" s="23"/>
       <c r="M31" s="10"/>
       <c r="N31" s="10"/>
-      <c r="O31" s="39"/>
+      <c r="O31" s="31"/>
       <c r="P31" s="1"/>
       <c r="Q31" s="1"/>
       <c r="R31" s="1"/>
@@ -2606,22 +2617,22 @@
       <c r="AE31" s="1"/>
       <c r="AF31" s="1"/>
     </row>
-    <row r="32" spans="1:32">
+    <row r="32" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
-      <c r="B32" s="24"/>
+      <c r="B32" s="16"/>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
-      <c r="E32" s="33"/>
+      <c r="E32" s="25"/>
       <c r="F32" s="7"/>
-      <c r="G32" s="26"/>
+      <c r="G32" s="18"/>
       <c r="H32" s="7"/>
       <c r="I32" s="7"/>
-      <c r="J32" s="37"/>
+      <c r="J32" s="29"/>
       <c r="K32" s="10"/>
-      <c r="L32" s="31"/>
+      <c r="L32" s="23"/>
       <c r="M32" s="10"/>
       <c r="N32" s="10"/>
-      <c r="O32" s="39"/>
+      <c r="O32" s="31"/>
       <c r="P32" s="1"/>
       <c r="Q32" s="1"/>
       <c r="R32" s="1"/>
@@ -2640,22 +2651,22 @@
       <c r="AE32" s="1"/>
       <c r="AF32" s="1"/>
     </row>
-    <row r="33" spans="1:32">
+    <row r="33" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
-      <c r="B33" s="24"/>
+      <c r="B33" s="16"/>
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
-      <c r="E33" s="33"/>
+      <c r="E33" s="25"/>
       <c r="F33" s="7"/>
-      <c r="G33" s="26"/>
+      <c r="G33" s="18"/>
       <c r="H33" s="7"/>
       <c r="I33" s="7"/>
-      <c r="J33" s="37"/>
+      <c r="J33" s="29"/>
       <c r="K33" s="10"/>
-      <c r="L33" s="31"/>
+      <c r="L33" s="23"/>
       <c r="M33" s="10"/>
       <c r="N33" s="10"/>
-      <c r="O33" s="39"/>
+      <c r="O33" s="31"/>
       <c r="P33" s="1"/>
       <c r="Q33" s="1"/>
       <c r="R33" s="1"/>
@@ -2674,22 +2685,22 @@
       <c r="AE33" s="1"/>
       <c r="AF33" s="1"/>
     </row>
-    <row r="34" spans="1:32">
+    <row r="34" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
-      <c r="B34" s="24"/>
+      <c r="B34" s="16"/>
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
-      <c r="E34" s="33"/>
+      <c r="E34" s="25"/>
       <c r="F34" s="7"/>
-      <c r="G34" s="26"/>
+      <c r="G34" s="18"/>
       <c r="H34" s="7"/>
       <c r="I34" s="7"/>
-      <c r="J34" s="37"/>
+      <c r="J34" s="29"/>
       <c r="K34" s="10"/>
-      <c r="L34" s="31"/>
+      <c r="L34" s="23"/>
       <c r="M34" s="10"/>
       <c r="N34" s="10"/>
-      <c r="O34" s="39"/>
+      <c r="O34" s="31"/>
       <c r="P34" s="1"/>
       <c r="Q34" s="1"/>
       <c r="R34" s="1"/>
@@ -2708,22 +2719,22 @@
       <c r="AE34" s="1"/>
       <c r="AF34" s="1"/>
     </row>
-    <row r="35" spans="1:32">
+    <row r="35" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
-      <c r="B35" s="24"/>
+      <c r="B35" s="16"/>
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
-      <c r="E35" s="33"/>
+      <c r="E35" s="25"/>
       <c r="F35" s="7"/>
-      <c r="G35" s="26"/>
+      <c r="G35" s="18"/>
       <c r="H35" s="7"/>
       <c r="I35" s="7"/>
-      <c r="J35" s="37"/>
+      <c r="J35" s="29"/>
       <c r="K35" s="10"/>
-      <c r="L35" s="31"/>
+      <c r="L35" s="23"/>
       <c r="M35" s="10"/>
       <c r="N35" s="10"/>
-      <c r="O35" s="39"/>
+      <c r="O35" s="31"/>
       <c r="P35" s="1"/>
       <c r="Q35" s="1"/>
       <c r="R35" s="1"/>
@@ -2742,22 +2753,22 @@
       <c r="AE35" s="1"/>
       <c r="AF35" s="1"/>
     </row>
-    <row r="36" spans="1:32">
+    <row r="36" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
-      <c r="B36" s="24"/>
+      <c r="B36" s="16"/>
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>
-      <c r="E36" s="33"/>
+      <c r="E36" s="25"/>
       <c r="F36" s="7"/>
-      <c r="G36" s="26"/>
+      <c r="G36" s="18"/>
       <c r="H36" s="7"/>
       <c r="I36" s="7"/>
-      <c r="J36" s="37"/>
+      <c r="J36" s="29"/>
       <c r="K36" s="10"/>
-      <c r="L36" s="31"/>
+      <c r="L36" s="23"/>
       <c r="M36" s="10"/>
       <c r="N36" s="10"/>
-      <c r="O36" s="39"/>
+      <c r="O36" s="31"/>
       <c r="P36" s="1"/>
       <c r="Q36" s="1"/>
       <c r="R36" s="1"/>
@@ -2776,22 +2787,22 @@
       <c r="AE36" s="1"/>
       <c r="AF36" s="1"/>
     </row>
-    <row r="37" spans="1:32">
+    <row r="37" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
-      <c r="B37" s="24"/>
+      <c r="B37" s="16"/>
       <c r="C37" s="4"/>
       <c r="D37" s="4"/>
-      <c r="E37" s="33"/>
+      <c r="E37" s="25"/>
       <c r="F37" s="7"/>
-      <c r="G37" s="26"/>
+      <c r="G37" s="18"/>
       <c r="H37" s="7"/>
       <c r="I37" s="7"/>
-      <c r="J37" s="37"/>
+      <c r="J37" s="29"/>
       <c r="K37" s="10"/>
-      <c r="L37" s="31"/>
+      <c r="L37" s="23"/>
       <c r="M37" s="10"/>
       <c r="N37" s="10"/>
-      <c r="O37" s="39"/>
+      <c r="O37" s="31"/>
       <c r="P37" s="1"/>
       <c r="Q37" s="1"/>
       <c r="R37" s="1"/>
@@ -2810,22 +2821,22 @@
       <c r="AE37" s="1"/>
       <c r="AF37" s="1"/>
     </row>
-    <row r="38" spans="1:32">
+    <row r="38" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
-      <c r="B38" s="24"/>
+      <c r="B38" s="16"/>
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>
-      <c r="E38" s="33"/>
+      <c r="E38" s="25"/>
       <c r="F38" s="7"/>
-      <c r="G38" s="26"/>
+      <c r="G38" s="18"/>
       <c r="H38" s="7"/>
       <c r="I38" s="7"/>
-      <c r="J38" s="37"/>
+      <c r="J38" s="29"/>
       <c r="K38" s="10"/>
-      <c r="L38" s="31"/>
+      <c r="L38" s="23"/>
       <c r="M38" s="10"/>
       <c r="N38" s="10"/>
-      <c r="O38" s="39"/>
+      <c r="O38" s="31"/>
       <c r="P38" s="1"/>
       <c r="Q38" s="1"/>
       <c r="R38" s="1"/>
@@ -2844,22 +2855,22 @@
       <c r="AE38" s="1"/>
       <c r="AF38" s="1"/>
     </row>
-    <row r="39" spans="1:32">
+    <row r="39" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
-      <c r="B39" s="24"/>
+      <c r="B39" s="16"/>
       <c r="C39" s="4"/>
       <c r="D39" s="4"/>
-      <c r="E39" s="33"/>
+      <c r="E39" s="25"/>
       <c r="F39" s="7"/>
-      <c r="G39" s="26"/>
+      <c r="G39" s="18"/>
       <c r="H39" s="7"/>
       <c r="I39" s="7"/>
-      <c r="J39" s="37"/>
+      <c r="J39" s="29"/>
       <c r="K39" s="10"/>
-      <c r="L39" s="31"/>
+      <c r="L39" s="23"/>
       <c r="M39" s="10"/>
       <c r="N39" s="10"/>
-      <c r="O39" s="39"/>
+      <c r="O39" s="31"/>
       <c r="P39" s="1"/>
       <c r="Q39" s="1"/>
       <c r="R39" s="1"/>
@@ -2878,22 +2889,22 @@
       <c r="AE39" s="1"/>
       <c r="AF39" s="1"/>
     </row>
-    <row r="40" spans="1:32">
+    <row r="40" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
-      <c r="B40" s="24"/>
+      <c r="B40" s="16"/>
       <c r="C40" s="4"/>
       <c r="D40" s="4"/>
-      <c r="E40" s="33"/>
+      <c r="E40" s="25"/>
       <c r="F40" s="7"/>
-      <c r="G40" s="26"/>
+      <c r="G40" s="18"/>
       <c r="H40" s="7"/>
       <c r="I40" s="7"/>
-      <c r="J40" s="37"/>
+      <c r="J40" s="29"/>
       <c r="K40" s="10"/>
-      <c r="L40" s="31"/>
+      <c r="L40" s="23"/>
       <c r="M40" s="10"/>
       <c r="N40" s="10"/>
-      <c r="O40" s="39"/>
+      <c r="O40" s="31"/>
       <c r="P40" s="1"/>
       <c r="Q40" s="1"/>
       <c r="R40" s="1"/>
@@ -2912,22 +2923,22 @@
       <c r="AE40" s="1"/>
       <c r="AF40" s="1"/>
     </row>
-    <row r="41" spans="1:32">
+    <row r="41" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A41" s="4"/>
-      <c r="B41" s="24"/>
+      <c r="B41" s="16"/>
       <c r="C41" s="4"/>
       <c r="D41" s="4"/>
-      <c r="E41" s="33"/>
+      <c r="E41" s="25"/>
       <c r="F41" s="7"/>
-      <c r="G41" s="26"/>
+      <c r="G41" s="18"/>
       <c r="H41" s="7"/>
       <c r="I41" s="7"/>
-      <c r="J41" s="37"/>
+      <c r="J41" s="29"/>
       <c r="K41" s="10"/>
-      <c r="L41" s="31"/>
+      <c r="L41" s="23"/>
       <c r="M41" s="10"/>
       <c r="N41" s="10"/>
-      <c r="O41" s="39"/>
+      <c r="O41" s="31"/>
       <c r="P41" s="1"/>
       <c r="Q41" s="1"/>
       <c r="R41" s="1"/>
@@ -2946,22 +2957,22 @@
       <c r="AE41" s="1"/>
       <c r="AF41" s="1"/>
     </row>
-    <row r="42" spans="1:32">
+    <row r="42" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
-      <c r="B42" s="24"/>
+      <c r="B42" s="16"/>
       <c r="C42" s="4"/>
       <c r="D42" s="4"/>
-      <c r="E42" s="33"/>
+      <c r="E42" s="25"/>
       <c r="F42" s="7"/>
-      <c r="G42" s="26"/>
+      <c r="G42" s="18"/>
       <c r="H42" s="7"/>
       <c r="I42" s="7"/>
-      <c r="J42" s="37"/>
+      <c r="J42" s="29"/>
       <c r="K42" s="10"/>
-      <c r="L42" s="31"/>
+      <c r="L42" s="23"/>
       <c r="M42" s="10"/>
       <c r="N42" s="10"/>
-      <c r="O42" s="39"/>
+      <c r="O42" s="31"/>
       <c r="P42" s="1"/>
       <c r="Q42" s="1"/>
       <c r="R42" s="1"/>
@@ -2980,22 +2991,22 @@
       <c r="AE42" s="1"/>
       <c r="AF42" s="1"/>
     </row>
-    <row r="43" spans="1:32">
+    <row r="43" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A43" s="4"/>
-      <c r="B43" s="24"/>
+      <c r="B43" s="16"/>
       <c r="C43" s="4"/>
       <c r="D43" s="4"/>
-      <c r="E43" s="33"/>
+      <c r="E43" s="25"/>
       <c r="F43" s="7"/>
-      <c r="G43" s="26"/>
+      <c r="G43" s="18"/>
       <c r="H43" s="7"/>
       <c r="I43" s="7"/>
-      <c r="J43" s="37"/>
+      <c r="J43" s="29"/>
       <c r="K43" s="10"/>
-      <c r="L43" s="31"/>
+      <c r="L43" s="23"/>
       <c r="M43" s="10"/>
       <c r="N43" s="10"/>
-      <c r="O43" s="39"/>
+      <c r="O43" s="31"/>
       <c r="P43" s="1"/>
       <c r="Q43" s="1"/>
       <c r="R43" s="1"/>
@@ -3014,22 +3025,22 @@
       <c r="AE43" s="1"/>
       <c r="AF43" s="1"/>
     </row>
-    <row r="44" spans="1:32">
+    <row r="44" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A44" s="4"/>
-      <c r="B44" s="24"/>
+      <c r="B44" s="16"/>
       <c r="C44" s="4"/>
       <c r="D44" s="4"/>
-      <c r="E44" s="33"/>
+      <c r="E44" s="25"/>
       <c r="F44" s="7"/>
-      <c r="G44" s="26"/>
+      <c r="G44" s="18"/>
       <c r="H44" s="7"/>
       <c r="I44" s="7"/>
-      <c r="J44" s="37"/>
+      <c r="J44" s="29"/>
       <c r="K44" s="10"/>
-      <c r="L44" s="31"/>
+      <c r="L44" s="23"/>
       <c r="M44" s="10"/>
       <c r="N44" s="10"/>
-      <c r="O44" s="39"/>
+      <c r="O44" s="31"/>
       <c r="P44" s="1"/>
       <c r="Q44" s="1"/>
       <c r="R44" s="1"/>
@@ -3048,22 +3059,22 @@
       <c r="AE44" s="1"/>
       <c r="AF44" s="1"/>
     </row>
-    <row r="45" spans="1:32">
+    <row r="45" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A45" s="4"/>
-      <c r="B45" s="24"/>
+      <c r="B45" s="16"/>
       <c r="C45" s="4"/>
       <c r="D45" s="4"/>
-      <c r="E45" s="33"/>
+      <c r="E45" s="25"/>
       <c r="F45" s="7"/>
-      <c r="G45" s="26"/>
+      <c r="G45" s="18"/>
       <c r="H45" s="7"/>
       <c r="I45" s="7"/>
-      <c r="J45" s="37"/>
+      <c r="J45" s="29"/>
       <c r="K45" s="10"/>
-      <c r="L45" s="31"/>
+      <c r="L45" s="23"/>
       <c r="M45" s="10"/>
       <c r="N45" s="10"/>
-      <c r="O45" s="39"/>
+      <c r="O45" s="31"/>
       <c r="P45" s="1"/>
       <c r="Q45" s="1"/>
       <c r="R45" s="1"/>
@@ -3082,22 +3093,22 @@
       <c r="AE45" s="1"/>
       <c r="AF45" s="1"/>
     </row>
-    <row r="46" spans="1:32">
+    <row r="46" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
-      <c r="B46" s="27"/>
+      <c r="B46" s="19"/>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
-      <c r="E46" s="34"/>
+      <c r="E46" s="26"/>
       <c r="F46" s="1"/>
-      <c r="G46" s="27"/>
+      <c r="G46" s="19"/>
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
-      <c r="J46" s="34"/>
+      <c r="J46" s="26"/>
       <c r="K46" s="1"/>
-      <c r="L46" s="27"/>
+      <c r="L46" s="19"/>
       <c r="M46" s="1"/>
       <c r="N46" s="1"/>
-      <c r="O46" s="34"/>
+      <c r="O46" s="26"/>
       <c r="P46" s="1"/>
       <c r="Q46" s="1"/>
       <c r="R46" s="1"/>
@@ -3116,22 +3127,22 @@
       <c r="AE46" s="1"/>
       <c r="AF46" s="1"/>
     </row>
-    <row r="47" spans="1:32">
+    <row r="47" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
-      <c r="B47" s="27"/>
+      <c r="B47" s="19"/>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
-      <c r="E47" s="34"/>
+      <c r="E47" s="26"/>
       <c r="F47" s="1"/>
-      <c r="G47" s="27"/>
+      <c r="G47" s="19"/>
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
-      <c r="J47" s="34"/>
+      <c r="J47" s="26"/>
       <c r="K47" s="1"/>
-      <c r="L47" s="27"/>
+      <c r="L47" s="19"/>
       <c r="M47" s="1"/>
       <c r="N47" s="1"/>
-      <c r="O47" s="34"/>
+      <c r="O47" s="26"/>
       <c r="P47" s="1"/>
       <c r="Q47" s="1"/>
       <c r="R47" s="1"/>
@@ -3174,95 +3185,95 @@
       <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
-      <c r="A2" s="20" t="s">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
-      <c r="A3" s="21" t="s">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
-      <c r="A4" s="21" t="s">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
-      <c r="A5" s="21" t="s">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
-      <c r="A6" s="21" t="s">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
-      <c r="A7" s="20" t="s">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
-      <c r="A8" s="21" t="s">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
-      <c r="A9" s="22" t="s">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
-      <c r="A10" s="21" t="s">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
-      <c r="A11" s="21" t="s">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="13" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
-      <c r="A12" s="20" t="s">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="12" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:1">
-      <c r="A13" s="21" t="s">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="13" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:1">
-      <c r="A14" s="21" t="s">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="13" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:1">
-      <c r="A15" s="20" t="s">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="12" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:1">
-      <c r="A16" s="22" t="s">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="14" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
-      <c r="A17" s="21" t="s">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="13" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
-      <c r="A18" s="23"/>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>